<commit_message>
Cambios Ubi - PB
</commit_message>
<xml_diff>
--- a/Documentation/Product Backlog - GreenPoint.xlsx
+++ b/Documentation/Product Backlog - GreenPoint.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liveespochedu-my.sharepoint.com/personal/cristhian_totoy_espoch_edu_ec/Documents/Espoch/8° Semestre/Aplicaciones Informaticas II/GreenPoint/GreenPoint/Documentation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\OCTAVO SEMESTRE\APLICACIONES INFORMÁTICAS II\GreenPoint\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{81BCE08E-FF4D-42EB-AE22-11FC9FD52E80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0607329B-3C90-43F6-B494-025224FAFADF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D50759C3-BA45-48EB-BAE2-5D7B3BF8F4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -327,9 +327,6 @@
     <t>Con la finalidad de registrar el punto verde de mi negocio en la app.</t>
   </si>
   <si>
-    <t>Necesito visualizar los clientes registrados en mi negocio</t>
-  </si>
-  <si>
     <t>Con la finalidad agilizar el proceso de registro de reciclaje por parte de clientes que han acudido anteriormente.</t>
   </si>
   <si>
@@ -423,9 +420,6 @@
     <t>10/07/2024 -16/07/2025</t>
   </si>
   <si>
-    <t>17/07/2024 23/07/2026</t>
-  </si>
-  <si>
     <t>Desarrollo de Endpoints CRUD</t>
   </si>
   <si>
@@ -523,6 +517,12 @@
   </si>
   <si>
     <t>rec_grenc</t>
+  </si>
+  <si>
+    <t>17/07/2024 21/07/2026</t>
+  </si>
+  <si>
+    <t>Necesito visualizar historial de clientes que reciclaron en mi negocio</t>
   </si>
 </sst>
 </file>
@@ -642,7 +642,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -717,11 +717,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -800,6 +813,14 @@
     <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -836,10 +857,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1131,32 +1148,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BF120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView topLeftCell="A9" zoomScale="80" zoomScaleNormal="80" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.453125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16.453125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.44140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="63" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="2" customWidth="1"/>
     <col min="5" max="5" width="11" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="13.1796875" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9.453125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.21875" style="2" customWidth="1"/>
+    <col min="8" max="8" width="9.44140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="73" style="2" customWidth="1"/>
-    <col min="10" max="10" width="5.08984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="4.08984375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.90625" style="2" customWidth="1"/>
-    <col min="13" max="13" width="86.90625" style="2" customWidth="1"/>
+    <col min="10" max="10" width="5.109375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="4.109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="8.88671875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="86.88671875" style="2" customWidth="1"/>
     <col min="14" max="14" width="3" style="2" customWidth="1"/>
-    <col min="15" max="15" width="11.453125" style="2"/>
-    <col min="16" max="16" width="24.90625" style="2" customWidth="1"/>
-    <col min="17" max="16384" width="11.453125" style="2"/>
+    <col min="15" max="15" width="11.44140625" style="2"/>
+    <col min="16" max="16" width="24.88671875" style="2" customWidth="1"/>
+    <col min="17" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:58" ht="36" x14ac:dyDescent="0.8">
+    <row r="1" spans="2:58" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B1" s="3" t="s">
         <v>4</v>
       </c>
@@ -1174,7 +1191,7 @@
       <c r="V1"/>
       <c r="W1"/>
     </row>
-    <row r="2" spans="2:58" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:58" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="4"/>
       <c r="K2"/>
       <c r="L2"/>
@@ -1190,7 +1207,7 @@
       <c r="V2"/>
       <c r="W2"/>
     </row>
-    <row r="3" spans="2:58" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:58" x14ac:dyDescent="0.3">
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
@@ -1205,7 +1222,7 @@
       <c r="V3"/>
       <c r="W3"/>
     </row>
-    <row r="4" spans="2:58" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="2:58" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
@@ -1244,7 +1261,7 @@
       <c r="V4"/>
       <c r="W4"/>
     </row>
-    <row r="5" spans="2:58" ht="53" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="2:58" ht="52.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="8" t="s">
         <v>48</v>
       </c>
@@ -1252,16 +1269,16 @@
         <v>64</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F5" s="8">
         <v>2</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>36</v>
@@ -1278,10 +1295,10 @@
       </c>
       <c r="N5"/>
       <c r="O5" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="P5" s="17" t="s">
         <v>116</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>117</v>
       </c>
       <c r="Q5"/>
       <c r="R5"/>
@@ -1291,7 +1308,7 @@
       <c r="V5"/>
       <c r="W5"/>
     </row>
-    <row r="6" spans="2:58" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="2:58" ht="54" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="8" t="s">
         <v>49</v>
       </c>
@@ -1299,16 +1316,16 @@
         <v>66</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F6" s="8">
         <v>3</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H6" s="8" t="s">
         <v>36</v>
@@ -1328,7 +1345,7 @@
         <v>47</v>
       </c>
       <c r="P6" s="18" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="Q6"/>
       <c r="R6"/>
@@ -1338,7 +1355,7 @@
       <c r="V6"/>
       <c r="W6"/>
     </row>
-    <row r="7" spans="2:58" ht="46.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="2:58" ht="46.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B7" s="8" t="s">
         <v>50</v>
       </c>
@@ -1346,10 +1363,10 @@
         <v>68</v>
       </c>
       <c r="D7" s="22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F7" s="8">
         <v>3</v>
@@ -1375,7 +1392,7 @@
         <v>46</v>
       </c>
       <c r="P7" s="18" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="Q7"/>
       <c r="R7"/>
@@ -1385,18 +1402,18 @@
       <c r="V7"/>
       <c r="W7"/>
     </row>
-    <row r="8" spans="2:58" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:58" ht="50.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D8" s="22" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F8" s="8">
         <v>4</v>
@@ -1422,7 +1439,7 @@
         <v>39</v>
       </c>
       <c r="P8" s="18" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="Q8"/>
       <c r="R8"/>
@@ -1432,16 +1449,16 @@
       <c r="V8"/>
       <c r="W8"/>
     </row>
-    <row r="9" spans="2:58" ht="52.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:58" ht="52.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="16"/>
       <c r="C9" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F9" s="7">
         <v>2</v>
@@ -1453,7 +1470,7 @@
         <v>36</v>
       </c>
       <c r="I9" s="21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="K9"/>
       <c r="L9" s="12">
@@ -1467,7 +1484,7 @@
         <v>40</v>
       </c>
       <c r="P9" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="Q9"/>
       <c r="R9"/>
@@ -1477,7 +1494,7 @@
       <c r="V9"/>
       <c r="W9"/>
     </row>
-    <row r="10" spans="2:58" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="10" spans="2:58" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="8" t="s">
         <v>51</v>
       </c>
@@ -1485,10 +1502,10 @@
         <v>72</v>
       </c>
       <c r="D10" s="22" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F10" s="8">
         <v>4</v>
@@ -1514,7 +1531,7 @@
         <v>41</v>
       </c>
       <c r="P10" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="Q10"/>
       <c r="R10"/>
@@ -1524,7 +1541,7 @@
       <c r="V10"/>
       <c r="W10"/>
     </row>
-    <row r="11" spans="2:58" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:58" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="8" t="s">
         <v>21</v>
       </c>
@@ -1532,10 +1549,10 @@
         <v>84</v>
       </c>
       <c r="D11" s="22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F11" s="8">
         <v>3</v>
@@ -1557,7 +1574,7 @@
         <v>42</v>
       </c>
       <c r="P11" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="Q11"/>
       <c r="R11"/>
@@ -1567,7 +1584,7 @@
       <c r="V11"/>
       <c r="W11"/>
     </row>
-    <row r="12" spans="2:58" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:58" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="8" t="s">
         <v>25</v>
       </c>
@@ -1575,10 +1592,10 @@
         <v>83</v>
       </c>
       <c r="D12" s="22" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F12" s="7">
         <v>2</v>
@@ -1598,7 +1615,7 @@
         <v>43</v>
       </c>
       <c r="P12" s="18" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="Q12"/>
       <c r="R12"/>
@@ -1608,18 +1625,18 @@
       <c r="V12"/>
       <c r="W12"/>
     </row>
-    <row r="13" spans="2:58" ht="33" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:58" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D13" s="22" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F13" s="7">
         <v>2</v>
@@ -1631,7 +1648,7 @@
         <v>36</v>
       </c>
       <c r="I13" s="21" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="K13"/>
       <c r="L13"/>
@@ -1641,7 +1658,7 @@
         <v>37</v>
       </c>
       <c r="P13" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="Q13"/>
       <c r="R13"/>
@@ -1651,7 +1668,7 @@
       <c r="V13"/>
       <c r="W13"/>
     </row>
-    <row r="14" spans="2:58" ht="34.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:58" ht="34.200000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="8" t="s">
         <v>32</v>
       </c>
@@ -1659,10 +1676,10 @@
         <v>70</v>
       </c>
       <c r="D14" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F14" s="8">
         <v>3</v>
@@ -1680,11 +1697,11 @@
       <c r="L14"/>
       <c r="M14"/>
       <c r="N14"/>
-      <c r="O14" s="9" t="s">
+      <c r="O14" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="P14" s="18" t="s">
-        <v>125</v>
+      <c r="P14" s="31" t="s">
+        <v>157</v>
       </c>
       <c r="Q14"/>
       <c r="R14"/>
@@ -1694,7 +1711,7 @@
       <c r="V14"/>
       <c r="W14"/>
     </row>
-    <row r="15" spans="2:58" ht="46.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:58" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="8" t="s">
         <v>22</v>
       </c>
@@ -1702,10 +1719,10 @@
         <v>75</v>
       </c>
       <c r="D15" s="22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="7" t="s">
@@ -1717,21 +1734,21 @@
       <c r="I15" s="19" t="s">
         <v>76</v>
       </c>
-      <c r="K15"/>
-      <c r="L15"/>
-      <c r="M15"/>
-      <c r="N15"/>
-      <c r="O15"/>
-      <c r="P15"/>
-      <c r="Q15"/>
-      <c r="R15"/>
-      <c r="S15"/>
-      <c r="T15"/>
+      <c r="K15" s="32"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="32"/>
+      <c r="Q15" s="32"/>
+      <c r="R15" s="32"/>
+      <c r="S15" s="32"/>
+      <c r="T15" s="32"/>
       <c r="U15"/>
       <c r="V15"/>
       <c r="W15"/>
     </row>
-    <row r="16" spans="2:58" ht="39.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:58" ht="39.450000000000003" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="8" t="s">
         <v>23</v>
       </c>
@@ -1739,10 +1756,10 @@
         <v>77</v>
       </c>
       <c r="D16" s="22" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="7" t="s">
@@ -1754,8 +1771,16 @@
       <c r="I16" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="K16"/>
-      <c r="L16"/>
+      <c r="K16" s="32"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="33"/>
+      <c r="N16" s="33"/>
+      <c r="O16" s="33"/>
+      <c r="P16" s="33"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="33"/>
+      <c r="S16" s="33"/>
+      <c r="T16" s="33"/>
       <c r="U16"/>
       <c r="V16"/>
       <c r="W16"/>
@@ -1795,7 +1820,7 @@
       <c r="BE16"/>
       <c r="BF16"/>
     </row>
-    <row r="17" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:58" ht="34.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="7" t="s">
         <v>26</v>
       </c>
@@ -1803,13 +1828,13 @@
         <v>86</v>
       </c>
       <c r="D17" s="22" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G17" s="7" t="s">
         <v>41</v>
@@ -1820,8 +1845,16 @@
       <c r="I17" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="K17"/>
-      <c r="T17"/>
+      <c r="K17" s="32"/>
+      <c r="L17" s="33"/>
+      <c r="M17" s="33"/>
+      <c r="N17" s="33"/>
+      <c r="O17" s="33"/>
+      <c r="P17" s="33"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="33"/>
+      <c r="S17" s="33"/>
+      <c r="T17" s="32"/>
       <c r="U17"/>
       <c r="V17"/>
       <c r="W17"/>
@@ -1861,7 +1894,7 @@
       <c r="BE17"/>
       <c r="BF17"/>
     </row>
-    <row r="18" spans="1:58" ht="34" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:58" ht="34.049999999999997" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="7" t="s">
         <v>27</v>
       </c>
@@ -1869,13 +1902,13 @@
         <v>88</v>
       </c>
       <c r="D18" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="G18" s="7" t="s">
         <v>41</v>
@@ -1886,16 +1919,16 @@
       <c r="I18" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="K18"/>
-      <c r="L18"/>
-      <c r="M18"/>
-      <c r="N18"/>
-      <c r="O18"/>
-      <c r="P18"/>
-      <c r="Q18"/>
-      <c r="R18"/>
-      <c r="S18"/>
-      <c r="T18"/>
+      <c r="K18" s="32"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="32"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="32"/>
+      <c r="R18" s="32"/>
+      <c r="S18" s="32"/>
+      <c r="T18" s="32"/>
       <c r="U18"/>
       <c r="V18"/>
       <c r="W18"/>
@@ -1935,18 +1968,18 @@
       <c r="BE18"/>
       <c r="BF18"/>
     </row>
-    <row r="19" spans="1:58" ht="30.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:58" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="8" t="s">
         <v>29</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>93</v>
+        <v>158</v>
       </c>
       <c r="D19" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="8"/>
       <c r="G19" s="7" t="s">
@@ -1956,18 +1989,18 @@
         <v>36</v>
       </c>
       <c r="I19" s="19" t="s">
-        <v>94</v>
-      </c>
-      <c r="K19"/>
-      <c r="L19"/>
-      <c r="M19"/>
-      <c r="N19"/>
-      <c r="O19"/>
-      <c r="P19"/>
-      <c r="Q19"/>
-      <c r="R19"/>
-      <c r="S19"/>
-      <c r="T19"/>
+        <v>93</v>
+      </c>
+      <c r="K19" s="32"/>
+      <c r="L19" s="32"/>
+      <c r="M19" s="32"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="32"/>
+      <c r="Q19" s="32"/>
+      <c r="R19" s="32"/>
+      <c r="S19" s="32"/>
+      <c r="T19" s="32"/>
       <c r="U19"/>
       <c r="V19"/>
       <c r="W19"/>
@@ -2007,7 +2040,7 @@
       <c r="BE19"/>
       <c r="BF19"/>
     </row>
-    <row r="20" spans="1:58" ht="48.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:58" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15" t="s">
         <v>52</v>
       </c>
@@ -2015,10 +2048,10 @@
         <v>79</v>
       </c>
       <c r="D20" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="7" t="s">
@@ -2071,7 +2104,7 @@
       <c r="BE20"/>
       <c r="BF20"/>
     </row>
-    <row r="21" spans="1:58" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:58" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="8" t="s">
         <v>24</v>
       </c>
@@ -2079,10 +2112,10 @@
         <v>81</v>
       </c>
       <c r="D21" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="7" t="s">
@@ -2143,18 +2176,18 @@
       <c r="BE21"/>
       <c r="BF21"/>
     </row>
-    <row r="22" spans="1:58" ht="29" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:58" ht="28.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="7" t="s">
         <v>30</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D22" s="22" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F22" s="7"/>
       <c r="G22" s="7" t="s">
@@ -2164,7 +2197,7 @@
         <v>36</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="J22"/>
       <c r="K22"/>
@@ -2216,18 +2249,18 @@
       <c r="BE22"/>
       <c r="BF22"/>
     </row>
-    <row r="23" spans="1:58" ht="32.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:58" ht="32.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="7" t="s">
         <v>45</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D23" s="22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="7" t="s">
@@ -2237,7 +2270,7 @@
         <v>36</v>
       </c>
       <c r="I23" s="19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J23"/>
       <c r="K23"/>
@@ -2289,7 +2322,7 @@
       <c r="BE23"/>
       <c r="BF23"/>
     </row>
-    <row r="24" spans="1:58" ht="49.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:58" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24"/>
       <c r="B24" s="8" t="s">
         <v>54</v>
@@ -2298,10 +2331,10 @@
         <v>53</v>
       </c>
       <c r="D24" s="22" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F24" s="8"/>
       <c r="G24" s="7" t="s">
@@ -2363,7 +2396,7 @@
       <c r="BE24"/>
       <c r="BF24"/>
     </row>
-    <row r="25" spans="1:58" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:58" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25"/>
       <c r="B25" s="10" t="s">
         <v>28</v>
@@ -2372,10 +2405,10 @@
         <v>91</v>
       </c>
       <c r="D25" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="7" t="s">
@@ -2437,19 +2470,19 @@
       <c r="BE25"/>
       <c r="BF25"/>
     </row>
-    <row r="26" spans="1:58" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:58" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26"/>
       <c r="B26" s="10" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="25" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D26" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F26" s="9"/>
       <c r="G26" s="7" t="s">
@@ -2459,7 +2492,7 @@
         <v>36</v>
       </c>
       <c r="I26" s="29" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="J26"/>
       <c r="K26"/>
@@ -2511,19 +2544,19 @@
       <c r="BE26"/>
       <c r="BF26"/>
     </row>
-    <row r="27" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:58" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27"/>
       <c r="B27" s="10" t="s">
         <v>34</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D27" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F27" s="9"/>
       <c r="G27" s="7" t="s">
@@ -2533,7 +2566,7 @@
         <v>36</v>
       </c>
       <c r="I27" s="29" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J27"/>
       <c r="K27"/>
@@ -2585,19 +2618,19 @@
       <c r="BE27"/>
       <c r="BF27"/>
     </row>
-    <row r="28" spans="1:58" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:58" ht="48" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28"/>
       <c r="B28" s="10" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D28" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
       <c r="F28" s="9"/>
       <c r="G28" s="7" t="s">
@@ -2607,7 +2640,7 @@
         <v>36</v>
       </c>
       <c r="I28" s="29" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="J28"/>
       <c r="K28"/>
@@ -2659,16 +2692,16 @@
       <c r="BE28"/>
       <c r="BF28"/>
     </row>
-    <row r="29" spans="1:58" ht="28.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:58" ht="28.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29"/>
       <c r="B29" s="10" t="s">
         <v>44</v>
       </c>
       <c r="C29" s="25" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D29" s="22" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>35</v>
@@ -2681,7 +2714,7 @@
         <v>36</v>
       </c>
       <c r="I29" s="29" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J29"/>
       <c r="K29"/>
@@ -2733,16 +2766,16 @@
       <c r="BE29"/>
       <c r="BF29"/>
     </row>
-    <row r="30" spans="1:58" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:58" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A30"/>
       <c r="B30" s="15" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D30" s="22" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E30" s="8" t="s">
         <v>35</v>
@@ -2755,7 +2788,7 @@
         <v>36</v>
       </c>
       <c r="I30" s="27" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J30"/>
       <c r="K30"/>
@@ -2807,16 +2840,16 @@
       <c r="BE30"/>
       <c r="BF30"/>
     </row>
-    <row r="31" spans="1:58" ht="40.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:58" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A31"/>
       <c r="B31" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D31" s="22" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>35</v>
@@ -2829,7 +2862,7 @@
         <v>36</v>
       </c>
       <c r="I31" s="27" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J31"/>
       <c r="K31"/>
@@ -2881,7 +2914,7 @@
       <c r="BE31"/>
       <c r="BF31"/>
     </row>
-    <row r="32" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A32"/>
       <c r="B32"/>
       <c r="C32"/>
@@ -2941,7 +2974,7 @@
       <c r="BE32"/>
       <c r="BF32"/>
     </row>
-    <row r="33" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A33"/>
       <c r="B33"/>
       <c r="C33"/>
@@ -3001,7 +3034,7 @@
       <c r="BE33"/>
       <c r="BF33"/>
     </row>
-    <row r="34" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A34"/>
       <c r="B34"/>
       <c r="C34"/>
@@ -3061,7 +3094,7 @@
       <c r="BE34"/>
       <c r="BF34"/>
     </row>
-    <row r="35" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A35"/>
       <c r="B35"/>
       <c r="C35"/>
@@ -3121,7 +3154,7 @@
       <c r="BE35"/>
       <c r="BF35"/>
     </row>
-    <row r="36" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A36"/>
       <c r="B36"/>
       <c r="C36"/>
@@ -3181,7 +3214,7 @@
       <c r="BE36"/>
       <c r="BF36"/>
     </row>
-    <row r="37" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A37"/>
       <c r="B37"/>
       <c r="C37"/>
@@ -3241,7 +3274,7 @@
       <c r="BE37"/>
       <c r="BF37"/>
     </row>
-    <row r="38" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A38"/>
       <c r="B38"/>
       <c r="C38"/>
@@ -3301,7 +3334,7 @@
       <c r="BE38"/>
       <c r="BF38"/>
     </row>
-    <row r="39" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A39"/>
       <c r="B39"/>
       <c r="C39"/>
@@ -3361,7 +3394,7 @@
       <c r="BE39"/>
       <c r="BF39"/>
     </row>
-    <row r="40" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A40"/>
       <c r="B40"/>
       <c r="C40"/>
@@ -3421,7 +3454,7 @@
       <c r="BE40"/>
       <c r="BF40"/>
     </row>
-    <row r="41" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A41"/>
       <c r="B41"/>
       <c r="C41"/>
@@ -3481,7 +3514,7 @@
       <c r="BE41"/>
       <c r="BF41"/>
     </row>
-    <row r="42" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A42"/>
       <c r="B42"/>
       <c r="C42"/>
@@ -3541,7 +3574,7 @@
       <c r="BE42"/>
       <c r="BF42"/>
     </row>
-    <row r="43" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A43"/>
       <c r="B43"/>
       <c r="C43"/>
@@ -3601,7 +3634,7 @@
       <c r="BE43"/>
       <c r="BF43"/>
     </row>
-    <row r="44" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A44"/>
       <c r="B44"/>
       <c r="C44"/>
@@ -3661,7 +3694,7 @@
       <c r="BE44"/>
       <c r="BF44"/>
     </row>
-    <row r="45" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A45"/>
       <c r="B45"/>
       <c r="C45"/>
@@ -3721,7 +3754,7 @@
       <c r="BE45"/>
       <c r="BF45"/>
     </row>
-    <row r="46" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A46"/>
       <c r="B46"/>
       <c r="C46"/>
@@ -3781,7 +3814,7 @@
       <c r="BE46"/>
       <c r="BF46"/>
     </row>
-    <row r="47" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A47"/>
       <c r="B47"/>
       <c r="C47"/>
@@ -3841,7 +3874,7 @@
       <c r="BE47"/>
       <c r="BF47"/>
     </row>
-    <row r="48" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A48"/>
       <c r="B48"/>
       <c r="C48"/>
@@ -3901,7 +3934,7 @@
       <c r="BE48"/>
       <c r="BF48"/>
     </row>
-    <row r="49" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A49"/>
       <c r="B49"/>
       <c r="C49"/>
@@ -3961,7 +3994,7 @@
       <c r="BE49"/>
       <c r="BF49"/>
     </row>
-    <row r="50" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A50"/>
       <c r="B50"/>
       <c r="C50"/>
@@ -4021,7 +4054,7 @@
       <c r="BE50"/>
       <c r="BF50"/>
     </row>
-    <row r="51" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A51"/>
       <c r="B51"/>
       <c r="C51"/>
@@ -4081,7 +4114,7 @@
       <c r="BE51"/>
       <c r="BF51"/>
     </row>
-    <row r="52" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A52"/>
       <c r="B52"/>
       <c r="C52"/>
@@ -4141,7 +4174,7 @@
       <c r="BE52"/>
       <c r="BF52"/>
     </row>
-    <row r="53" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A53"/>
       <c r="B53"/>
       <c r="C53"/>
@@ -4201,7 +4234,7 @@
       <c r="BE53"/>
       <c r="BF53"/>
     </row>
-    <row r="54" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A54"/>
       <c r="B54"/>
       <c r="C54"/>
@@ -4261,7 +4294,7 @@
       <c r="BE54"/>
       <c r="BF54"/>
     </row>
-    <row r="55" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A55"/>
       <c r="B55"/>
       <c r="C55"/>
@@ -4321,7 +4354,7 @@
       <c r="BE55"/>
       <c r="BF55"/>
     </row>
-    <row r="56" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A56"/>
       <c r="B56"/>
       <c r="C56"/>
@@ -4381,7 +4414,7 @@
       <c r="BE56"/>
       <c r="BF56"/>
     </row>
-    <row r="57" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A57"/>
       <c r="B57"/>
       <c r="C57"/>
@@ -4441,7 +4474,7 @@
       <c r="BE57"/>
       <c r="BF57"/>
     </row>
-    <row r="58" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A58"/>
       <c r="B58"/>
       <c r="C58"/>
@@ -4501,7 +4534,7 @@
       <c r="BE58"/>
       <c r="BF58"/>
     </row>
-    <row r="59" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A59"/>
       <c r="B59"/>
       <c r="C59"/>
@@ -4561,7 +4594,7 @@
       <c r="BE59"/>
       <c r="BF59"/>
     </row>
-    <row r="60" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A60"/>
       <c r="B60"/>
       <c r="C60"/>
@@ -4621,7 +4654,7 @@
       <c r="BE60"/>
       <c r="BF60"/>
     </row>
-    <row r="61" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A61"/>
       <c r="B61"/>
       <c r="C61"/>
@@ -4681,7 +4714,7 @@
       <c r="BE61"/>
       <c r="BF61"/>
     </row>
-    <row r="62" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A62"/>
       <c r="B62"/>
       <c r="C62"/>
@@ -4741,7 +4774,7 @@
       <c r="BE62"/>
       <c r="BF62"/>
     </row>
-    <row r="63" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A63"/>
       <c r="B63"/>
       <c r="C63"/>
@@ -4801,7 +4834,7 @@
       <c r="BE63"/>
       <c r="BF63"/>
     </row>
-    <row r="64" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A64"/>
       <c r="B64"/>
       <c r="C64"/>
@@ -4861,7 +4894,7 @@
       <c r="BE64"/>
       <c r="BF64"/>
     </row>
-    <row r="65" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A65"/>
       <c r="B65"/>
       <c r="C65"/>
@@ -4921,7 +4954,7 @@
       <c r="BE65"/>
       <c r="BF65"/>
     </row>
-    <row r="66" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A66"/>
       <c r="B66"/>
       <c r="C66"/>
@@ -4981,7 +5014,7 @@
       <c r="BE66"/>
       <c r="BF66"/>
     </row>
-    <row r="67" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A67"/>
       <c r="B67"/>
       <c r="C67"/>
@@ -5041,7 +5074,7 @@
       <c r="BE67"/>
       <c r="BF67"/>
     </row>
-    <row r="68" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A68"/>
       <c r="B68"/>
       <c r="C68"/>
@@ -5101,7 +5134,7 @@
       <c r="BE68"/>
       <c r="BF68"/>
     </row>
-    <row r="69" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A69"/>
       <c r="B69"/>
       <c r="C69"/>
@@ -5161,7 +5194,7 @@
       <c r="BE69"/>
       <c r="BF69"/>
     </row>
-    <row r="70" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A70"/>
       <c r="B70"/>
       <c r="C70"/>
@@ -5221,7 +5254,7 @@
       <c r="BE70"/>
       <c r="BF70"/>
     </row>
-    <row r="71" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A71"/>
       <c r="B71"/>
       <c r="C71"/>
@@ -5281,7 +5314,7 @@
       <c r="BE71"/>
       <c r="BF71"/>
     </row>
-    <row r="72" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A72"/>
       <c r="B72"/>
       <c r="C72"/>
@@ -5316,7 +5349,7 @@
       <c r="AF72"/>
       <c r="AG72"/>
     </row>
-    <row r="73" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A73"/>
       <c r="B73"/>
       <c r="C73"/>
@@ -5351,7 +5384,7 @@
       <c r="AF73"/>
       <c r="AG73"/>
     </row>
-    <row r="74" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A74"/>
       <c r="B74"/>
       <c r="C74"/>
@@ -5386,7 +5419,7 @@
       <c r="AF74"/>
       <c r="AG74"/>
     </row>
-    <row r="75" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A75"/>
       <c r="B75"/>
       <c r="C75"/>
@@ -5421,7 +5454,7 @@
       <c r="AF75"/>
       <c r="AG75"/>
     </row>
-    <row r="76" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A76"/>
       <c r="B76"/>
       <c r="C76"/>
@@ -5456,7 +5489,7 @@
       <c r="AF76"/>
       <c r="AG76"/>
     </row>
-    <row r="77" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A77"/>
       <c r="B77"/>
       <c r="C77"/>
@@ -5491,7 +5524,7 @@
       <c r="AF77"/>
       <c r="AG77"/>
     </row>
-    <row r="78" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A78"/>
       <c r="B78"/>
       <c r="C78"/>
@@ -5526,7 +5559,7 @@
       <c r="AF78"/>
       <c r="AG78"/>
     </row>
-    <row r="79" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A79"/>
       <c r="B79"/>
       <c r="C79"/>
@@ -5561,7 +5594,7 @@
       <c r="AF79"/>
       <c r="AG79"/>
     </row>
-    <row r="80" spans="1:58" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A80"/>
       <c r="B80"/>
       <c r="C80"/>
@@ -5596,7 +5629,7 @@
       <c r="AF80"/>
       <c r="AG80"/>
     </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A81"/>
       <c r="B81"/>
       <c r="C81"/>
@@ -5631,7 +5664,7 @@
       <c r="AF81"/>
       <c r="AG81"/>
     </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A82"/>
       <c r="B82"/>
       <c r="C82"/>
@@ -5666,7 +5699,7 @@
       <c r="AF82"/>
       <c r="AG82"/>
     </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A83"/>
       <c r="B83"/>
       <c r="C83"/>
@@ -5701,7 +5734,7 @@
       <c r="AF83"/>
       <c r="AG83"/>
     </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A84"/>
       <c r="B84"/>
       <c r="C84"/>
@@ -5736,7 +5769,7 @@
       <c r="AF84"/>
       <c r="AG84"/>
     </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A85"/>
       <c r="B85"/>
       <c r="C85"/>
@@ -5771,7 +5804,7 @@
       <c r="AF85"/>
       <c r="AG85"/>
     </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A86"/>
       <c r="B86"/>
       <c r="C86"/>
@@ -5806,7 +5839,7 @@
       <c r="AF86"/>
       <c r="AG86"/>
     </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A87"/>
       <c r="B87"/>
       <c r="C87"/>
@@ -5841,7 +5874,7 @@
       <c r="AF87"/>
       <c r="AG87"/>
     </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A88"/>
       <c r="B88"/>
       <c r="C88"/>
@@ -5876,7 +5909,7 @@
       <c r="AF88"/>
       <c r="AG88"/>
     </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A89"/>
       <c r="B89"/>
       <c r="C89"/>
@@ -5911,7 +5944,7 @@
       <c r="AF89"/>
       <c r="AG89"/>
     </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A90"/>
       <c r="B90"/>
       <c r="C90"/>
@@ -5946,7 +5979,7 @@
       <c r="AF90"/>
       <c r="AG90"/>
     </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A91"/>
       <c r="B91"/>
       <c r="C91"/>
@@ -5981,7 +6014,7 @@
       <c r="AF91"/>
       <c r="AG91"/>
     </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A92"/>
       <c r="B92"/>
       <c r="C92"/>
@@ -6016,7 +6049,7 @@
       <c r="AF92"/>
       <c r="AG92"/>
     </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A93"/>
       <c r="B93"/>
       <c r="C93"/>
@@ -6051,7 +6084,7 @@
       <c r="AF93"/>
       <c r="AG93"/>
     </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A94"/>
       <c r="B94"/>
       <c r="C94"/>
@@ -6086,7 +6119,7 @@
       <c r="AF94"/>
       <c r="AG94"/>
     </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A95"/>
       <c r="B95"/>
       <c r="C95"/>
@@ -6121,7 +6154,7 @@
       <c r="AF95"/>
       <c r="AG95"/>
     </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A96"/>
       <c r="B96"/>
       <c r="C96"/>
@@ -6156,7 +6189,7 @@
       <c r="AF96"/>
       <c r="AG96"/>
     </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A97"/>
       <c r="B97"/>
       <c r="C97"/>
@@ -6191,7 +6224,7 @@
       <c r="AF97"/>
       <c r="AG97"/>
     </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A98"/>
       <c r="B98"/>
       <c r="C98"/>
@@ -6226,7 +6259,7 @@
       <c r="AF98"/>
       <c r="AG98"/>
     </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A99"/>
       <c r="B99"/>
       <c r="C99"/>
@@ -6261,7 +6294,7 @@
       <c r="AF99"/>
       <c r="AG99"/>
     </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A100"/>
       <c r="B100"/>
       <c r="C100"/>
@@ -6296,7 +6329,7 @@
       <c r="AF100"/>
       <c r="AG100"/>
     </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A101"/>
       <c r="B101"/>
       <c r="C101"/>
@@ -6331,7 +6364,7 @@
       <c r="AF101"/>
       <c r="AG101"/>
     </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A102"/>
       <c r="B102"/>
       <c r="C102"/>
@@ -6366,7 +6399,7 @@
       <c r="AF102"/>
       <c r="AG102"/>
     </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A103"/>
       <c r="B103"/>
       <c r="C103"/>
@@ -6401,7 +6434,7 @@
       <c r="AF103"/>
       <c r="AG103"/>
     </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A104"/>
       <c r="B104"/>
       <c r="C104"/>
@@ -6436,7 +6469,7 @@
       <c r="AF104"/>
       <c r="AG104"/>
     </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A105"/>
       <c r="B105"/>
       <c r="C105"/>
@@ -6471,7 +6504,7 @@
       <c r="AF105"/>
       <c r="AG105"/>
     </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A106"/>
       <c r="B106"/>
       <c r="C106"/>
@@ -6506,7 +6539,7 @@
       <c r="AF106"/>
       <c r="AG106"/>
     </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A107"/>
       <c r="B107"/>
       <c r="C107"/>
@@ -6541,7 +6574,7 @@
       <c r="AF107"/>
       <c r="AG107"/>
     </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A108"/>
       <c r="B108"/>
       <c r="C108"/>
@@ -6576,7 +6609,7 @@
       <c r="AF108"/>
       <c r="AG108"/>
     </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A109"/>
       <c r="B109"/>
       <c r="C109"/>
@@ -6611,7 +6644,7 @@
       <c r="AF109"/>
       <c r="AG109"/>
     </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A110"/>
       <c r="B110"/>
       <c r="C110"/>
@@ -6646,7 +6679,7 @@
       <c r="AF110"/>
       <c r="AG110"/>
     </row>
-    <row r="111" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A111"/>
       <c r="B111"/>
       <c r="C111"/>
@@ -6681,7 +6714,7 @@
       <c r="AF111"/>
       <c r="AG111"/>
     </row>
-    <row r="112" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A112"/>
       <c r="B112"/>
       <c r="C112"/>
@@ -6716,7 +6749,7 @@
       <c r="AF112"/>
       <c r="AG112"/>
     </row>
-    <row r="113" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A113"/>
       <c r="B113"/>
       <c r="C113"/>
@@ -6751,7 +6784,7 @@
       <c r="AF113"/>
       <c r="AG113"/>
     </row>
-    <row r="114" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A114"/>
       <c r="B114"/>
       <c r="C114"/>
@@ -6786,7 +6819,7 @@
       <c r="AF114"/>
       <c r="AG114"/>
     </row>
-    <row r="115" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A115"/>
       <c r="B115"/>
       <c r="C115"/>
@@ -6821,7 +6854,7 @@
       <c r="AF115"/>
       <c r="AG115"/>
     </row>
-    <row r="116" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A116"/>
       <c r="B116"/>
       <c r="C116"/>
@@ -6856,7 +6889,7 @@
       <c r="AF116"/>
       <c r="AG116"/>
     </row>
-    <row r="117" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A117"/>
       <c r="B117"/>
       <c r="C117"/>
@@ -6891,7 +6924,7 @@
       <c r="AF117"/>
       <c r="AG117"/>
     </row>
-    <row r="118" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A118"/>
       <c r="B118"/>
       <c r="C118"/>
@@ -6926,7 +6959,7 @@
       <c r="AF118"/>
       <c r="AG118"/>
     </row>
-    <row r="119" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A119"/>
       <c r="B119"/>
       <c r="C119"/>
@@ -6961,7 +6994,7 @@
       <c r="AF119"/>
       <c r="AG119"/>
     </row>
-    <row r="120" spans="1:33" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A120"/>
       <c r="B120"/>
       <c r="C120"/>
@@ -7018,30 +7051,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:C12"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A2" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A2" zoomScale="70" zoomScaleSheetLayoutView="70" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.54296875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="27.81640625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="1.5546875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="27.77734375" style="2" customWidth="1"/>
     <col min="3" max="3" width="86" style="2" customWidth="1"/>
-    <col min="4" max="4" width="2.81640625" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="11.453125" style="2"/>
+    <col min="4" max="4" width="2.77734375" style="2" customWidth="1"/>
+    <col min="5" max="16384" width="11.44140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" ht="36" x14ac:dyDescent="0.8">
+    <row r="1" spans="2:3" ht="36.6" x14ac:dyDescent="0.7">
       <c r="B1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:3" ht="21" x14ac:dyDescent="0.4">
       <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -7049,7 +7082,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
@@ -7057,7 +7090,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="2:3" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" ht="72" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="s">
         <v>3</v>
       </c>
@@ -7065,7 +7098,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="2:3" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="s">
         <v>19</v>
       </c>
@@ -7073,7 +7106,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="2:3" ht="217.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" ht="187.2" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="s">
         <v>7</v>
       </c>
@@ -7081,7 +7114,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" ht="50.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="s">
         <v>8</v>
       </c>
@@ -7089,7 +7122,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="2:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
@@ -7097,7 +7130,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="2:3" ht="58" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B11" s="5" t="s">
         <v>10</v>
       </c>
@@ -7105,7 +7138,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="2:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B12" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>